<commit_message>
Deploying to pages from @ MAWoodMain/kicad-automation-test@9ef6d8ffc67c6650fd0c07450279509d2e60ecc0 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/kicad-automation-test-bom.xlsx
+++ b/BoM/Costs/kicad-automation-test-bom.xlsx
@@ -253,7 +253,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-02-10_23-25-35</t>
+    <t>2023-02-10_23-45-28</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -307,7 +307,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-02-10 23:25:44</t>
+    <t>2023-02-10 23:45:37</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.0</t>

</xml_diff>

<commit_message>
Deploying to pages from @ MAWoodMain/kicad-automation-test@2cccc0866fbe29276387f4969c0b005ccbc7b615 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/kicad-automation-test-bom.xlsx
+++ b/BoM/Costs/kicad-automation-test-bom.xlsx
@@ -253,7 +253,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-02-10_23-45-28</t>
+    <t>2023-02-10_23-49-14</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -307,7 +307,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-02-10 23:45:37</t>
+    <t>2023-02-10 23:49:24</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.0</t>

</xml_diff>